<commit_message>
changing to fit taxo report
</commit_message>
<xml_diff>
--- a/input/tpt_dwc_template.xlsx
+++ b/input/tpt_dwc_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A30E0BAA-82FF-4C0F-9073-5399E20D84CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{A30E0BAA-82FF-4C0F-9073-5399E20D84CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E918F133-49F8-4502-A985-6B3C1B0AA738}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ED67756A-F5D5-4E60-8843-DB3C0F0BF365}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
-  <si>
-    <t>TPTdataset</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>taxonID</t>
   </si>
@@ -138,7 +135,7 @@
     <t>taxonRemarks</t>
   </si>
   <si>
-    <t>TPTID</t>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -503,18 +500,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810D4FB4-3811-4750-B54C-17B5FE81B7AA}">
-  <dimension ref="A1:AR1"/>
+  <dimension ref="A1:AQ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -612,9 +609,7 @@
       <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
+      <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
@@ -623,7 +618,6 @@
       <c r="AO1" s="2"/>
       <c r="AP1" s="2"/>
       <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>